<commit_message>
Adjust sale price prediction
Price rises on 2017-4-18
</commit_message>
<xml_diff>
--- a/data-mining/models/SalePricePrediction.xlsx
+++ b/data-mining/models/SalePricePrediction.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i327636\Desktop\tmp\weka\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my-git\data-mining\DataMining\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D17711B-59A4-48B5-A147-935D916C34AC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3500CF56-B70A-4A47-B327-BF75A0B6A627}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{F5520AB2-0AAD-4727-A666-01A28D23D08C}"/>
   </bookViews>
@@ -391,8 +391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B6DD4AA-DD74-4C4C-A250-5F45E6769FE2}">
   <dimension ref="A1:C1082"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A1030" workbookViewId="0">
+      <selection activeCell="I1058" sqref="I1058"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9412,7 +9412,7 @@
         <v>42842</v>
       </c>
       <c r="C824">
-        <v>5.99</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="825" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>